<commit_message>
Update SCH to A4 page size
</commit_message>
<xml_diff>
--- a/FAB/BOM.xlsx
+++ b/FAB/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A552123\Documents\KiCad Projects\beginner_project_1\FAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A552123\Documents\Git\Personal\PacketVis_hardware\FAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DDBF02D-3EA8-4AD0-9B4C-D7B986A78E8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E30522-A566-4ABE-905E-5C38A8A3C40E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="-12795" windowWidth="11775" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t xml:space="preserve">    C1</t>
   </si>
@@ -196,6 +196,24 @@
   </si>
   <si>
     <t>https://www.espressif.com/sites/default/files/documentation/esp-wroom-02u_esp-wroom-02d_datasheet_en.pdf</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Manufacturer PN</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
   </si>
 </sst>
 </file>
@@ -656,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -672,30 +690,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -704,18 +722,18 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -724,18 +742,18 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -744,67 +762,67 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="E7">
-        <v>1050170001</v>
+      <c r="E7" t="s">
+        <v>21</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -812,47 +830,47 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
+      <c r="E8">
+        <v>1050170001</v>
+      </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -861,87 +879,87 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -949,21 +967,41 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>56</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>55</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>1</v>
       </c>
     </row>

</xml_diff>